<commit_message>
carga de app.py y requirements.txt
</commit_message>
<xml_diff>
--- a/etiquetas.xlsx
+++ b/etiquetas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbong\Documents\Proyectos\etiquetas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D22EE6-A3E6-4989-BBC9-48DCC1E9773D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1BE028-2D30-427B-8D1E-4400995FCA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="288" windowWidth="23232" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -225,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -241,10 +241,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -552,7 +549,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,7 +924,7 @@
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="1">

</xml_diff>